<commit_message>
Ret AD04 og ATD04b efter review
Coauthors: Toke and Emil
Reviewers: Daniel
</commit_message>
<xml_diff>
--- a/05 Test/ATD04b Angiv Salgsfremmende omkostninger.xlsx
+++ b/05 Test/ATD04b Angiv Salgsfremmende omkostninger.xlsx
@@ -56,7 +56,7 @@
     <t xml:space="preserve">Salgsfremmede omkostninger= -99,90 DDK</t>
   </si>
   <si>
-    <t xml:space="preserve">Negativ værdig</t>
+    <t xml:space="preserve">Failed with: Negativ værdig</t>
   </si>
 </sst>
 </file>
@@ -314,7 +314,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -407,15 +407,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -573,7 +565,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.67"/>
@@ -662,7 +654,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12"/>
-      <c r="B9" s="23"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,14 +664,14 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12"/>
-      <c r="B11" s="23"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24"/>
+      <c r="A16" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -707,386 +699,385 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="29.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="27.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="25" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="70.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="10" style="25" width="10.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="25" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="70.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="10" style="0" width="10.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="A3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="35"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="33"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="35"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="33"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="33"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="35"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="33"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="35"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="33"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="28"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="35"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="33"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="35"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="33"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="35"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="K13" s="36"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="33"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="K13" s="34"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="35"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="33"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="35"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="33"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27"/>
-      <c r="B18" s="37"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="35"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G20" s="31"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G21" s="31"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G22" s="31"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G23" s="31"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G24" s="31"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G25" s="31"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="31"/>
+      <c r="A26" s="24"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="26"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
+      <c r="B27" s="24"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G28" s="31"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G29" s="31"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G30" s="31"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G31" s="38"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G32" s="31"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="41"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="41"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="42"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="28"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="35"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="33"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="28"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="35"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="33"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="28"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="35"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="33"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="28"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="35"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="33"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="33"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="33"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
+      <c r="A53" s="31"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="33"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="31"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="28"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="28"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="35"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="33"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="28"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="28"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="35"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="33"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>